<commit_message>
New result: Extra Trees
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t xml:space="preserve">Nearest Centroid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extra Trees</t>
   </si>
 </sst>
 </file>
@@ -210,8 +213,8 @@
   </sheetPr>
   <dimension ref="A1:J518"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L32" activeCellId="0" sqref="L32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G66" activeCellId="0" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1192,144 +1195,72 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="0" t="n">
+      <c r="B34" s="1" t="n">
         <v>0.66</v>
       </c>
-      <c r="C34" s="0" t="n">
+      <c r="C34" s="1" t="n">
         <v>0.65</v>
       </c>
-      <c r="D34" s="0" t="n">
+      <c r="D34" s="1" t="n">
         <v>0.43</v>
       </c>
-      <c r="E34" s="0" t="n">
+      <c r="E34" s="1" t="n">
         <v>0.62</v>
       </c>
-      <c r="F34" s="0" t="n">
+      <c r="F34" s="1" t="n">
         <v>0.62</v>
       </c>
-      <c r="G34" s="0" t="n">
+      <c r="G34" s="1" t="n">
         <v>0.69</v>
       </c>
-      <c r="H34" s="0" t="n">
+      <c r="H34" s="1" t="n">
         <v>0.63</v>
       </c>
-      <c r="I34" s="0" t="n">
+      <c r="I34" s="1" t="n">
         <v>0.57</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-    </row>
-    <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-    </row>
-    <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-    </row>
-    <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-    </row>
-    <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-    </row>
-    <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-    </row>
-    <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-    </row>
+      <c r="A35" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <v>0.94</v>
+      </c>
+      <c r="H35" s="0" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="I35" s="0" t="n">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1656,154 +1587,154 @@
     <row r="368" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="369" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="370" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="373" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="374" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="375" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="382" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="396" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="397" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="398" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="399" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="400" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="401" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="402" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="403" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="407" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="408" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="409" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="411" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="413" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="414" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="415" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="416" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="417" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="418" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="422" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="423" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="424" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="425" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="427" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="432" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="433" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="434" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="436" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="448" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="457" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="467" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="486" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="487" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="488" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="489" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="490" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="491" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="492" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="493" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="495" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="496" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="502" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="506" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="507" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="508" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="509" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="510" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="511" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="512" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="513" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="514" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="515" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="516" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="517" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="518" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="371" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="372" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="373" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="374" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="375" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="376" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="377" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="378" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="379" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="380" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="381" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="382" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="383" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="384" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="385" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="386" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="387" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="388" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="389" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="390" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="391" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="392" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="393" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="394" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="395" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="396" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="397" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="398" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="399" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="400" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="401" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="402" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="403" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="404" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="405" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="406" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="407" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="408" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="409" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="410" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="411" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="412" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="413" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="414" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="415" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="416" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="417" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="418" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="419" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="420" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="421" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="422" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="423" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="424" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="425" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="426" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="427" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="428" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="429" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="430" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="431" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="432" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="433" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="434" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="435" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="436" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="437" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="438" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="439" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="440" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="441" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="442" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="443" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="444" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="445" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="446" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="447" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="448" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="449" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="450" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="451" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="452" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="453" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="454" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="455" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="456" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="457" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="458" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="459" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="460" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="461" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="462" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="463" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="464" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="465" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="466" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="467" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="468" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="469" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="470" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="471" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="472" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="473" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="474" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="475" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="476" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="477" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="478" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="479" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="480" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="481" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="482" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="483" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="484" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="485" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="486" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="487" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="488" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="489" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="490" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="491" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="492" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="493" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="494" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="495" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="496" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="497" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="498" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="499" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="500" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="501" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="502" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="503" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="504" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="505" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="506" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="507" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="508" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="509" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="510" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="511" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="512" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="513" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="514" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="515" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="516" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="517" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="518" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Bootstrapping results for the model: Extra Trees
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -213,8 +213,8 @@
   </sheetPr>
   <dimension ref="A1:J518"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G66" activeCellId="0" sqref="G66"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E43" activeCellId="0" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1224,40 +1224,100 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="0" t="n">
-        <v>0.93</v>
-      </c>
-      <c r="C35" s="0" t="n">
-        <v>0.93</v>
-      </c>
-      <c r="D35" s="0" t="n">
+      <c r="B35" s="1" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="D35" s="1" t="n">
         <v>0.87</v>
       </c>
-      <c r="E35" s="0" t="n">
-        <v>0.93</v>
-      </c>
-      <c r="F35" s="0" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="G35" s="0" t="n">
+      <c r="E35" s="1" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="G35" s="1" t="n">
         <v>0.94</v>
       </c>
-      <c r="H35" s="0" t="n">
-        <v>0.93</v>
-      </c>
-      <c r="I35" s="0" t="n">
-        <v>0.91</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="H35" s="1" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="I35" s="1" t="n">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+    </row>
     <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>